<commit_message>
Rerunning s/p removing IS from features
</commit_message>
<xml_diff>
--- a/output_demos_correlation_table.xlsx
+++ b/output_demos_correlation_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,21 +463,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000108-94-1_group1</t>
+          <t>000100-41-4_group4</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.14</v>
+        <v>-0.082</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.157</v>
+        <v>-0.076</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.044</v>
+        <v>0.037</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Possibly</t>
+          <t>Unlikely</t>
         </is>
       </c>
     </row>
@@ -488,13 +488,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.067</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.051</v>
+        <v>-0.004</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.008999999999999999</v>
+        <v>0.004</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -505,17 +505,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>002216-33-3_group1</t>
+          <t>000124-19-6_group1</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.017</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.01</v>
+        <v>0.008</v>
       </c>
       <c r="D4" t="n">
-        <v>0.014</v>
+        <v>0.01</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -526,40 +526,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>063521-76-6_group3</t>
+          <t>000098-86-2_group2</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.121</v>
+        <v>0.098</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.041</v>
+        <v>0.061</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.117</v>
+        <v>0.002</v>
       </c>
       <c r="E5" t="inlineStr">
-        <is>
-          <t>Unlikely</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1000308-17-8_group1</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.026</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.033</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-0.027</v>
-      </c>
-      <c r="E6" t="inlineStr">
         <is>
           <t>Unlikely</t>
         </is>

</xml_diff>

<commit_message>
removing TEL similar compound
</commit_message>
<xml_diff>
--- a/output_demos_correlation_table.xlsx
+++ b/output_demos_correlation_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000100-41-4_group4</t>
+          <t>000074-95-3_group1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.082</v>
+        <v>0.134</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.076</v>
+        <v>-0.1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.037</v>
+        <v>0.048</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -484,17 +484,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000110-88-3_group1</t>
+          <t>000098-86-2_group2</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.004</v>
+        <v>0.065</v>
       </c>
       <c r="D3" t="n">
-        <v>0.004</v>
+        <v>0.007</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -505,17 +505,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>000124-19-6_group1</t>
+          <t>001640-89-7_group2</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.07099999999999999</v>
+        <v>-0.053</v>
       </c>
       <c r="C4" t="n">
-        <v>0.008</v>
+        <v>0.02</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01</v>
+        <v>-0.08799999999999999</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -526,19 +526,145 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>000098-86-2_group2</t>
+          <t>002216-33-3_group1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.098</v>
+        <v>-0.038</v>
       </c>
       <c r="C5" t="n">
-        <v>0.061</v>
+        <v>0.017</v>
       </c>
       <c r="D5" t="n">
-        <v>0.002</v>
+        <v>-0.07099999999999999</v>
       </c>
       <c r="E5" t="inlineStr">
+        <is>
+          <t>Unlikely</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>000098-83-9_group2</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-0.067</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.08400000000000001</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.017</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Unlikely</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>000124-19-6_group1</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-0.018</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Unlikely</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>000620-14-4_group1</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.08699999999999999</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.092</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-0.045</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Unlikely</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>000095-16-9_group2</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.106</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-0.044</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Unlikely</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>000115-11-7_group2</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-0.019</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-0.058</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Unlikely</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>000617-94-7_group1</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-0.114</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>Unlikely</t>
         </is>

</xml_diff>

<commit_message>
Inclusion of TEL Similar Compound
</commit_message>
<xml_diff>
--- a/output_demos_correlation_table.xlsx
+++ b/output_demos_correlation_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000074-95-3_group1</t>
+          <t>000124-19-6_group1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.134</v>
+        <v>0.098</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1</v>
+        <v>0.029</v>
       </c>
       <c r="D2" t="n">
-        <v>0.048</v>
+        <v>0.01</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -484,17 +484,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000098-86-2_group2</t>
+          <t>1000401-12-0_group1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.121</v>
       </c>
       <c r="C3" t="n">
-        <v>0.065</v>
+        <v>-0.137</v>
       </c>
       <c r="D3" t="n">
-        <v>0.007</v>
+        <v>-0.106</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -505,17 +505,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>001640-89-7_group2</t>
+          <t>000615-74-7_group1</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.053</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="C4" t="n">
-        <v>0.02</v>
+        <v>0.132</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.08799999999999999</v>
+        <v>-0.045</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -526,17 +526,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>002216-33-3_group1</t>
+          <t>000098-86-2_group2</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.038</v>
+        <v>0.105</v>
       </c>
       <c r="C5" t="n">
-        <v>0.017</v>
+        <v>0.081</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.07099999999999999</v>
+        <v>-0.001</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -547,17 +547,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>000098-83-9_group2</t>
+          <t>1000309-13-0_group1</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.067</v>
+        <v>-0.034</v>
       </c>
       <c r="C6" t="n">
-        <v>0.08400000000000001</v>
+        <v>-0.026</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.017</v>
+        <v>-0.09</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -568,17 +568,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>000124-19-6_group1</t>
+          <t>054446-78-5_group1</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.051</v>
+        <v>0.048</v>
       </c>
       <c r="C7" t="n">
-        <v>0.033</v>
+        <v>0.055</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.018</v>
+        <v>-0.044</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -593,78 +593,15 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.103</v>
       </c>
       <c r="C8" t="n">
-        <v>0.092</v>
+        <v>0.046</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.045</v>
+        <v>-0.038</v>
       </c>
       <c r="E8" t="inlineStr">
-        <is>
-          <t>Unlikely</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>000095-16-9_group2</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>-0.106</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.031</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-0.044</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Unlikely</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>000115-11-7_group2</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>-0.019</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.099</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-0.058</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Unlikely</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>000617-94-7_group1</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>-0.114</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.008</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.039</v>
-      </c>
-      <c r="E11" t="inlineStr">
         <is>
           <t>Unlikely</t>
         </is>

</xml_diff>